<commit_message>
- Added: #34 Thêm chức năng chọn địa chỉ từ ô combobox
</commit_message>
<xml_diff>
--- a/database/files/Input_HCM.xlsx
+++ b/database/files/Input_HCM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Members" sheetId="1" r:id="rId1"/>
@@ -8129,7 +8129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U345"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
@@ -26256,12 +26256,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K352" sqref="K352"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -26335,7 +26334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" hidden="1">
+    <row r="2" spans="1:16" ht="16.5">
       <c r="A2" s="96">
         <v>1</v>
       </c>
@@ -26371,7 +26370,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" hidden="1">
+    <row r="3" spans="1:16" ht="16.5">
       <c r="A3" s="96">
         <v>2</v>
       </c>
@@ -26408,7 +26407,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" hidden="1">
+    <row r="4" spans="1:16" ht="16.5">
       <c r="A4" s="96">
         <v>3</v>
       </c>
@@ -26444,7 +26443,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5" hidden="1">
+    <row r="5" spans="1:16" ht="16.5">
       <c r="A5" s="96">
         <v>4</v>
       </c>
@@ -26480,7 +26479,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" hidden="1">
+    <row r="6" spans="1:16" ht="16.5">
       <c r="A6" s="96">
         <v>5</v>
       </c>
@@ -26516,7 +26515,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.5" hidden="1">
+    <row r="7" spans="1:16" ht="16.5">
       <c r="A7" s="96">
         <v>6</v>
       </c>
@@ -26550,7 +26549,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" hidden="1">
+    <row r="8" spans="1:16" ht="16.5">
       <c r="A8" s="96">
         <v>7</v>
       </c>
@@ -26584,7 +26583,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.5" hidden="1">
+    <row r="9" spans="1:16" ht="16.5">
       <c r="A9" s="96">
         <v>8</v>
       </c>
@@ -26620,7 +26619,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.5" hidden="1">
+    <row r="10" spans="1:16" ht="16.5">
       <c r="A10" s="96">
         <v>9</v>
       </c>
@@ -26656,7 +26655,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.5" hidden="1">
+    <row r="11" spans="1:16" ht="16.5">
       <c r="A11" s="96">
         <v>10</v>
       </c>
@@ -26692,7 +26691,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.5" hidden="1">
+    <row r="12" spans="1:16" ht="16.5">
       <c r="A12" s="96">
         <v>11</v>
       </c>
@@ -26728,7 +26727,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5" hidden="1">
+    <row r="13" spans="1:16" ht="16.5">
       <c r="A13" s="96">
         <v>12</v>
       </c>
@@ -26764,7 +26763,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" hidden="1">
+    <row r="14" spans="1:16" ht="16.5">
       <c r="A14" s="96">
         <v>13</v>
       </c>
@@ -26800,7 +26799,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16.5" hidden="1">
+    <row r="15" spans="1:16" ht="16.5">
       <c r="A15" s="96">
         <v>14</v>
       </c>
@@ -26836,7 +26835,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5" hidden="1">
+    <row r="16" spans="1:16" ht="16.5">
       <c r="A16" s="96">
         <v>15</v>
       </c>
@@ -26872,7 +26871,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16.5" hidden="1">
+    <row r="17" spans="1:14" ht="16.5">
       <c r="A17" s="96">
         <v>16</v>
       </c>
@@ -26908,7 +26907,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16.5" hidden="1">
+    <row r="18" spans="1:14" ht="16.5">
       <c r="A18" s="96">
         <v>17</v>
       </c>
@@ -26944,7 +26943,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.5" hidden="1">
+    <row r="19" spans="1:14" ht="16.5">
       <c r="A19" s="96">
         <v>18</v>
       </c>
@@ -26980,7 +26979,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16.5" hidden="1">
+    <row r="20" spans="1:14" ht="16.5">
       <c r="A20" s="96">
         <v>19</v>
       </c>
@@ -27016,7 +27015,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.5" hidden="1">
+    <row r="21" spans="1:14" ht="16.5">
       <c r="A21" s="96">
         <v>20</v>
       </c>
@@ -27052,7 +27051,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.5" hidden="1">
+    <row r="22" spans="1:14" ht="16.5">
       <c r="A22" s="96">
         <v>21</v>
       </c>
@@ -27088,7 +27087,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16.5" hidden="1">
+    <row r="23" spans="1:14" ht="16.5">
       <c r="A23" s="96">
         <v>22</v>
       </c>
@@ -27124,7 +27123,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16.5" hidden="1">
+    <row r="24" spans="1:14" ht="16.5">
       <c r="A24" s="96">
         <v>23</v>
       </c>
@@ -27160,7 +27159,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16.5" hidden="1">
+    <row r="25" spans="1:14" ht="16.5">
       <c r="A25" s="96">
         <v>24</v>
       </c>
@@ -27196,7 +27195,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16.5" hidden="1">
+    <row r="26" spans="1:14" ht="16.5">
       <c r="A26" s="96">
         <v>25</v>
       </c>
@@ -27232,7 +27231,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16.5" hidden="1">
+    <row r="27" spans="1:14" ht="16.5">
       <c r="A27" s="96">
         <v>26</v>
       </c>
@@ -27268,7 +27267,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.5" hidden="1">
+    <row r="28" spans="1:14" ht="16.5">
       <c r="A28" s="96">
         <v>27</v>
       </c>
@@ -27304,7 +27303,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.5" hidden="1">
+    <row r="29" spans="1:14" ht="16.5">
       <c r="A29" s="96">
         <v>28</v>
       </c>
@@ -27340,7 +27339,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.5" hidden="1">
+    <row r="30" spans="1:14" ht="16.5">
       <c r="A30" s="96">
         <v>29</v>
       </c>
@@ -27376,7 +27375,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.5" hidden="1">
+    <row r="31" spans="1:14" ht="16.5">
       <c r="A31" s="96">
         <v>30</v>
       </c>
@@ -27412,7 +27411,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.5" hidden="1">
+    <row r="32" spans="1:14" ht="16.5">
       <c r="A32" s="96">
         <v>31</v>
       </c>
@@ -27448,7 +27447,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.5" hidden="1">
+    <row r="33" spans="1:14" ht="16.5">
       <c r="A33" s="96">
         <v>32</v>
       </c>
@@ -27484,7 +27483,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.5" hidden="1">
+    <row r="34" spans="1:14" ht="16.5">
       <c r="A34" s="96">
         <v>33</v>
       </c>
@@ -27520,7 +27519,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.5" hidden="1">
+    <row r="35" spans="1:14" ht="16.5">
       <c r="A35" s="96">
         <v>34</v>
       </c>
@@ -27556,7 +27555,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.5" hidden="1">
+    <row r="36" spans="1:14" ht="16.5">
       <c r="A36" s="96">
         <v>35</v>
       </c>
@@ -27592,7 +27591,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.5" hidden="1">
+    <row r="37" spans="1:14" ht="16.5">
       <c r="A37" s="96">
         <v>36</v>
       </c>
@@ -27628,7 +27627,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.5" hidden="1">
+    <row r="38" spans="1:14" ht="16.5">
       <c r="A38" s="96">
         <v>37</v>
       </c>
@@ -27664,7 +27663,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.5" hidden="1">
+    <row r="39" spans="1:14" ht="16.5">
       <c r="A39" s="96">
         <v>38</v>
       </c>
@@ -27700,7 +27699,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16.5" hidden="1">
+    <row r="40" spans="1:14" ht="16.5">
       <c r="A40" s="96">
         <v>39</v>
       </c>
@@ -27736,7 +27735,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.5" hidden="1">
+    <row r="41" spans="1:14" ht="16.5">
       <c r="A41" s="96">
         <v>40</v>
       </c>
@@ -27772,7 +27771,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16.5" hidden="1">
+    <row r="42" spans="1:14" ht="16.5">
       <c r="A42" s="96">
         <v>41</v>
       </c>
@@ -27808,7 +27807,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16.5" hidden="1">
+    <row r="43" spans="1:14" ht="16.5">
       <c r="A43" s="96">
         <v>42</v>
       </c>
@@ -27844,7 +27843,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16.5" hidden="1">
+    <row r="44" spans="1:14" ht="16.5">
       <c r="A44" s="96">
         <v>43</v>
       </c>
@@ -27880,7 +27879,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.5" hidden="1">
+    <row r="45" spans="1:14" ht="16.5">
       <c r="A45" s="96">
         <v>44</v>
       </c>
@@ -27916,7 +27915,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16.5" hidden="1">
+    <row r="46" spans="1:14" ht="16.5">
       <c r="A46" s="96">
         <v>45</v>
       </c>
@@ -27952,7 +27951,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16.5" hidden="1">
+    <row r="47" spans="1:14" ht="16.5">
       <c r="A47" s="96">
         <v>46</v>
       </c>
@@ -27988,7 +27987,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16.5" hidden="1">
+    <row r="48" spans="1:14" ht="16.5">
       <c r="A48" s="96">
         <v>47</v>
       </c>
@@ -28024,7 +28023,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16.5" hidden="1">
+    <row r="49" spans="1:14" ht="16.5">
       <c r="A49" s="96">
         <v>48</v>
       </c>
@@ -28060,7 +28059,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16.5" hidden="1">
+    <row r="50" spans="1:14" ht="16.5">
       <c r="A50" s="96">
         <v>49</v>
       </c>
@@ -28096,7 +28095,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16.5" hidden="1">
+    <row r="51" spans="1:14" ht="16.5">
       <c r="A51" s="96">
         <v>50</v>
       </c>
@@ -28132,7 +28131,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16.5" hidden="1">
+    <row r="52" spans="1:14" ht="16.5">
       <c r="A52" s="96">
         <v>51</v>
       </c>
@@ -28168,7 +28167,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16.5" hidden="1">
+    <row r="53" spans="1:14" ht="16.5">
       <c r="A53" s="96">
         <v>52</v>
       </c>
@@ -28204,7 +28203,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="16.5" hidden="1">
+    <row r="54" spans="1:14" ht="16.5">
       <c r="A54" s="96">
         <v>53</v>
       </c>
@@ -28240,7 +28239,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="16.5" hidden="1">
+    <row r="55" spans="1:14" ht="16.5">
       <c r="A55" s="96">
         <v>54</v>
       </c>
@@ -28276,7 +28275,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16.5" hidden="1">
+    <row r="56" spans="1:14" ht="16.5">
       <c r="A56" s="96">
         <v>55</v>
       </c>
@@ -28312,7 +28311,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="16.5" hidden="1">
+    <row r="57" spans="1:14" ht="16.5">
       <c r="A57" s="96">
         <v>56</v>
       </c>
@@ -28348,7 +28347,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16.5" hidden="1">
+    <row r="58" spans="1:14" ht="16.5">
       <c r="A58" s="96">
         <v>57</v>
       </c>
@@ -28384,7 +28383,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="16.5" hidden="1">
+    <row r="59" spans="1:14" ht="16.5">
       <c r="A59" s="96">
         <v>58</v>
       </c>
@@ -28420,7 +28419,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="16.5" hidden="1">
+    <row r="60" spans="1:14" ht="16.5">
       <c r="A60" s="96">
         <v>59</v>
       </c>
@@ -28456,7 +28455,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="16.5" hidden="1">
+    <row r="61" spans="1:14" ht="16.5">
       <c r="A61" s="96">
         <v>60</v>
       </c>
@@ -28492,7 +28491,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="16.5" hidden="1">
+    <row r="62" spans="1:14" ht="16.5">
       <c r="A62" s="96">
         <v>61</v>
       </c>
@@ -28528,7 +28527,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="16.5" hidden="1">
+    <row r="63" spans="1:14" ht="16.5">
       <c r="A63" s="96">
         <v>62</v>
       </c>
@@ -28564,7 +28563,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="16.5" hidden="1">
+    <row r="64" spans="1:14" ht="16.5">
       <c r="A64" s="96">
         <v>63</v>
       </c>
@@ -28600,7 +28599,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="16.5" hidden="1">
+    <row r="65" spans="1:14" ht="16.5">
       <c r="A65" s="96">
         <v>64</v>
       </c>
@@ -28636,7 +28635,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="16.5" hidden="1">
+    <row r="66" spans="1:14" ht="16.5">
       <c r="A66" s="96">
         <v>65</v>
       </c>
@@ -28672,7 +28671,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="16.5" hidden="1">
+    <row r="67" spans="1:14" ht="16.5">
       <c r="A67" s="96">
         <v>66</v>
       </c>
@@ -28708,7 +28707,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="16.5" hidden="1">
+    <row r="68" spans="1:14" ht="16.5">
       <c r="A68" s="96">
         <v>67</v>
       </c>
@@ -28744,7 +28743,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="16.5" hidden="1">
+    <row r="69" spans="1:14" ht="16.5">
       <c r="A69" s="96">
         <v>68</v>
       </c>
@@ -28780,7 +28779,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="16.5" hidden="1">
+    <row r="70" spans="1:14" ht="16.5">
       <c r="A70" s="96">
         <v>69</v>
       </c>
@@ -28816,7 +28815,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="16.5" hidden="1">
+    <row r="71" spans="1:14" ht="16.5">
       <c r="A71" s="96">
         <v>70</v>
       </c>
@@ -28852,7 +28851,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="16.5" hidden="1">
+    <row r="72" spans="1:14" ht="16.5">
       <c r="A72" s="96">
         <v>71</v>
       </c>
@@ -28888,7 +28887,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="16.5" hidden="1">
+    <row r="73" spans="1:14" ht="16.5">
       <c r="A73" s="96">
         <v>72</v>
       </c>
@@ -28924,7 +28923,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="16.5" hidden="1">
+    <row r="74" spans="1:14" ht="16.5">
       <c r="A74" s="96">
         <v>73</v>
       </c>
@@ -28960,7 +28959,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="16.5" hidden="1">
+    <row r="75" spans="1:14" ht="16.5">
       <c r="A75" s="96">
         <v>74</v>
       </c>
@@ -28996,7 +28995,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="16.5" hidden="1">
+    <row r="76" spans="1:14" ht="16.5">
       <c r="A76" s="96">
         <v>75</v>
       </c>
@@ -29032,7 +29031,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="16.5" hidden="1">
+    <row r="77" spans="1:14" ht="16.5">
       <c r="A77" s="96">
         <v>76</v>
       </c>
@@ -29068,7 +29067,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="16.5" hidden="1">
+    <row r="78" spans="1:14" ht="16.5">
       <c r="A78" s="96">
         <v>77</v>
       </c>
@@ -29104,7 +29103,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="16.5" hidden="1">
+    <row r="79" spans="1:14" ht="16.5">
       <c r="A79" s="96">
         <v>78</v>
       </c>
@@ -29140,7 +29139,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="16.5" hidden="1">
+    <row r="80" spans="1:14" ht="16.5">
       <c r="A80" s="96">
         <v>79</v>
       </c>
@@ -29176,7 +29175,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="16.5" hidden="1">
+    <row r="81" spans="1:14" ht="16.5">
       <c r="A81" s="96">
         <v>80</v>
       </c>
@@ -29212,7 +29211,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="16.5" hidden="1">
+    <row r="82" spans="1:14" ht="16.5">
       <c r="A82" s="96">
         <v>81</v>
       </c>
@@ -29248,7 +29247,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="16.5" hidden="1">
+    <row r="83" spans="1:14" ht="16.5">
       <c r="A83" s="96">
         <v>82</v>
       </c>
@@ -29284,7 +29283,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="16.5" hidden="1">
+    <row r="84" spans="1:14" ht="16.5">
       <c r="A84" s="96">
         <v>83</v>
       </c>
@@ -29320,7 +29319,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="16.5" hidden="1">
+    <row r="85" spans="1:14" ht="16.5">
       <c r="A85" s="96">
         <v>84</v>
       </c>
@@ -29356,7 +29355,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="16.5" hidden="1">
+    <row r="86" spans="1:14" ht="16.5">
       <c r="A86" s="96">
         <v>85</v>
       </c>
@@ -29392,7 +29391,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="16.5" hidden="1">
+    <row r="87" spans="1:14" ht="16.5">
       <c r="A87" s="96">
         <v>86</v>
       </c>
@@ -29428,7 +29427,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="16.5" hidden="1">
+    <row r="88" spans="1:14" ht="16.5">
       <c r="A88" s="96">
         <v>87</v>
       </c>
@@ -29464,7 +29463,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="16.5" hidden="1">
+    <row r="89" spans="1:14" ht="16.5">
       <c r="A89" s="96">
         <v>88</v>
       </c>
@@ -29500,7 +29499,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="16.5" hidden="1">
+    <row r="90" spans="1:14" ht="16.5">
       <c r="A90" s="96">
         <v>89</v>
       </c>
@@ -29536,7 +29535,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="16.5" hidden="1">
+    <row r="91" spans="1:14" ht="16.5">
       <c r="A91" s="96">
         <v>90</v>
       </c>
@@ -29572,7 +29571,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="16.5" hidden="1">
+    <row r="92" spans="1:14" ht="16.5">
       <c r="A92" s="96">
         <v>91</v>
       </c>
@@ -29608,7 +29607,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="16.5" hidden="1">
+    <row r="93" spans="1:14" ht="16.5">
       <c r="A93" s="96">
         <v>92</v>
       </c>
@@ -29644,7 +29643,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="16.5" hidden="1">
+    <row r="94" spans="1:14" ht="16.5">
       <c r="A94" s="96">
         <v>93</v>
       </c>
@@ -29680,7 +29679,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="16.5" hidden="1">
+    <row r="95" spans="1:14" ht="16.5">
       <c r="A95" s="96">
         <v>94</v>
       </c>
@@ -29716,7 +29715,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="16.5" hidden="1">
+    <row r="96" spans="1:14" ht="16.5">
       <c r="A96" s="96">
         <v>95</v>
       </c>
@@ -29752,7 +29751,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="16.5" hidden="1">
+    <row r="97" spans="1:14" ht="16.5">
       <c r="A97" s="96">
         <v>96</v>
       </c>
@@ -29788,7 +29787,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="16.5" hidden="1">
+    <row r="98" spans="1:14" ht="16.5">
       <c r="A98" s="96">
         <v>97</v>
       </c>
@@ -29824,7 +29823,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="16.5" hidden="1">
+    <row r="99" spans="1:14" ht="16.5">
       <c r="A99" s="96">
         <v>98</v>
       </c>
@@ -29860,7 +29859,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="16.5" hidden="1">
+    <row r="100" spans="1:14" ht="16.5">
       <c r="A100" s="96">
         <v>99</v>
       </c>
@@ -29896,7 +29895,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="16.5" hidden="1">
+    <row r="101" spans="1:14" ht="16.5">
       <c r="A101" s="96">
         <v>100</v>
       </c>
@@ -29932,7 +29931,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="16.5" hidden="1">
+    <row r="102" spans="1:14" ht="16.5">
       <c r="A102" s="96">
         <v>101</v>
       </c>
@@ -29968,7 +29967,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="16.5" hidden="1">
+    <row r="103" spans="1:14" ht="16.5">
       <c r="A103" s="96">
         <v>102</v>
       </c>
@@ -30004,7 +30003,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="16.5" hidden="1">
+    <row r="104" spans="1:14" ht="16.5">
       <c r="A104" s="96">
         <v>103</v>
       </c>
@@ -30040,7 +30039,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="16.5" hidden="1">
+    <row r="105" spans="1:14" ht="16.5">
       <c r="A105" s="96">
         <v>104</v>
       </c>
@@ -30076,7 +30075,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="16.5" hidden="1">
+    <row r="106" spans="1:14" ht="16.5">
       <c r="A106" s="96">
         <v>105</v>
       </c>
@@ -30112,7 +30111,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="16.5" hidden="1">
+    <row r="107" spans="1:14" ht="16.5">
       <c r="A107" s="96">
         <v>106</v>
       </c>
@@ -30148,7 +30147,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="16.5" hidden="1">
+    <row r="108" spans="1:14" ht="16.5">
       <c r="A108" s="96">
         <v>107</v>
       </c>
@@ -30174,7 +30173,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="16.5" hidden="1">
+    <row r="109" spans="1:14" ht="16.5">
       <c r="A109" s="96">
         <v>108</v>
       </c>
@@ -30210,7 +30209,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="16.5" hidden="1">
+    <row r="110" spans="1:14" ht="16.5">
       <c r="A110" s="96">
         <v>109</v>
       </c>
@@ -30246,7 +30245,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="16.5" hidden="1">
+    <row r="111" spans="1:14" ht="16.5">
       <c r="A111" s="96">
         <v>110</v>
       </c>
@@ -30282,7 +30281,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="16.5" hidden="1">
+    <row r="112" spans="1:14" ht="16.5">
       <c r="A112" s="96">
         <v>111</v>
       </c>
@@ -30318,7 +30317,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="16.5" hidden="1">
+    <row r="113" spans="1:14" ht="16.5">
       <c r="A113" s="96">
         <v>112</v>
       </c>
@@ -30354,7 +30353,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="16.5" hidden="1">
+    <row r="114" spans="1:14" ht="16.5">
       <c r="A114" s="96">
         <v>113</v>
       </c>
@@ -30390,7 +30389,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="16.5" hidden="1">
+    <row r="115" spans="1:14" ht="16.5">
       <c r="A115" s="96">
         <v>114</v>
       </c>
@@ -30426,7 +30425,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="16.5" hidden="1">
+    <row r="116" spans="1:14" ht="16.5">
       <c r="A116" s="96">
         <v>115</v>
       </c>
@@ -30462,7 +30461,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="16.5" hidden="1">
+    <row r="117" spans="1:14" ht="16.5">
       <c r="A117" s="96">
         <v>116</v>
       </c>
@@ -30498,7 +30497,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="16.5" hidden="1">
+    <row r="118" spans="1:14" ht="16.5">
       <c r="A118" s="96">
         <v>117</v>
       </c>
@@ -30534,7 +30533,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="16.5" hidden="1">
+    <row r="119" spans="1:14" ht="16.5">
       <c r="A119" s="96">
         <v>118</v>
       </c>
@@ -30570,7 +30569,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="16.5" hidden="1">
+    <row r="120" spans="1:14" ht="16.5">
       <c r="A120" s="96">
         <v>119</v>
       </c>
@@ -30606,7 +30605,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="16.5" hidden="1">
+    <row r="121" spans="1:14" ht="16.5">
       <c r="A121" s="96">
         <v>120</v>
       </c>
@@ -30642,7 +30641,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="16.5" hidden="1">
+    <row r="122" spans="1:14" ht="16.5">
       <c r="A122" s="96">
         <v>121</v>
       </c>
@@ -30678,7 +30677,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="16.5" hidden="1">
+    <row r="123" spans="1:14" ht="16.5">
       <c r="A123" s="96">
         <v>122</v>
       </c>
@@ -30714,7 +30713,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="16.5" hidden="1">
+    <row r="124" spans="1:14" ht="16.5">
       <c r="A124" s="96">
         <v>123</v>
       </c>
@@ -30750,7 +30749,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="16.5" hidden="1">
+    <row r="125" spans="1:14" ht="16.5">
       <c r="A125" s="96">
         <v>124</v>
       </c>
@@ -30786,7 +30785,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="16.5" hidden="1">
+    <row r="126" spans="1:14" ht="16.5">
       <c r="A126" s="96">
         <v>125</v>
       </c>
@@ -30822,7 +30821,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="16.5" hidden="1">
+    <row r="127" spans="1:14" ht="16.5">
       <c r="A127" s="96">
         <v>126</v>
       </c>
@@ -30858,7 +30857,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="16.5" hidden="1">
+    <row r="128" spans="1:14" ht="16.5">
       <c r="A128" s="96">
         <v>127</v>
       </c>
@@ -30894,7 +30893,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="16.5" hidden="1">
+    <row r="129" spans="1:14" ht="16.5">
       <c r="A129" s="96">
         <v>128</v>
       </c>
@@ -30930,7 +30929,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="16.5" hidden="1">
+    <row r="130" spans="1:14" ht="16.5">
       <c r="A130" s="96">
         <v>129</v>
       </c>
@@ -30966,7 +30965,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="16.5" hidden="1">
+    <row r="131" spans="1:14" ht="16.5">
       <c r="A131" s="96">
         <v>130</v>
       </c>
@@ -31002,7 +31001,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="16.5" hidden="1">
+    <row r="132" spans="1:14" ht="16.5">
       <c r="A132" s="96">
         <v>131</v>
       </c>
@@ -31038,7 +31037,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="16.5" hidden="1">
+    <row r="133" spans="1:14" ht="16.5">
       <c r="A133" s="96">
         <v>132</v>
       </c>
@@ -31074,7 +31073,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="16.5" hidden="1">
+    <row r="134" spans="1:14" ht="16.5">
       <c r="A134" s="96">
         <v>133</v>
       </c>
@@ -31110,7 +31109,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="16.5" hidden="1">
+    <row r="135" spans="1:14" ht="16.5">
       <c r="A135" s="96">
         <v>134</v>
       </c>
@@ -31146,7 +31145,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="16.5" hidden="1">
+    <row r="136" spans="1:14" ht="16.5">
       <c r="A136" s="96">
         <v>135</v>
       </c>
@@ -31182,7 +31181,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="16.5" hidden="1">
+    <row r="137" spans="1:14" ht="16.5">
       <c r="A137" s="96">
         <v>136</v>
       </c>
@@ -31218,7 +31217,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="16.5" hidden="1">
+    <row r="138" spans="1:14" ht="16.5">
       <c r="A138" s="96">
         <v>137</v>
       </c>
@@ -31254,7 +31253,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="16.5" hidden="1">
+    <row r="139" spans="1:14" ht="16.5">
       <c r="A139" s="96">
         <v>138</v>
       </c>
@@ -31290,7 +31289,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="16.5" hidden="1">
+    <row r="140" spans="1:14" ht="16.5">
       <c r="A140" s="96">
         <v>139</v>
       </c>
@@ -31326,7 +31325,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="16.5" hidden="1">
+    <row r="141" spans="1:14" ht="16.5">
       <c r="A141" s="96">
         <v>140</v>
       </c>
@@ -31362,7 +31361,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="16.5" hidden="1">
+    <row r="142" spans="1:14" ht="16.5">
       <c r="A142" s="96">
         <v>141</v>
       </c>
@@ -31398,7 +31397,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="16.5" hidden="1">
+    <row r="143" spans="1:14" ht="16.5">
       <c r="A143" s="96">
         <v>142</v>
       </c>
@@ -31434,7 +31433,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="16.5" hidden="1">
+    <row r="144" spans="1:14" ht="16.5">
       <c r="A144" s="96">
         <v>143</v>
       </c>
@@ -31470,7 +31469,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="16.5" hidden="1">
+    <row r="145" spans="1:14" ht="16.5">
       <c r="A145" s="96">
         <v>144</v>
       </c>
@@ -31506,7 +31505,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="16.5" hidden="1">
+    <row r="146" spans="1:14" ht="16.5">
       <c r="A146" s="96">
         <v>145</v>
       </c>
@@ -31542,7 +31541,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="16.5" hidden="1">
+    <row r="147" spans="1:14" ht="16.5">
       <c r="A147" s="96">
         <v>146</v>
       </c>
@@ -31578,7 +31577,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="16.5" hidden="1">
+    <row r="148" spans="1:14" ht="16.5">
       <c r="A148" s="96">
         <v>147</v>
       </c>
@@ -31614,7 +31613,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="16.5" hidden="1">
+    <row r="149" spans="1:14" ht="16.5">
       <c r="A149" s="96">
         <v>148</v>
       </c>
@@ -31650,7 +31649,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="16.5" hidden="1">
+    <row r="150" spans="1:14" ht="16.5">
       <c r="A150" s="96">
         <v>149</v>
       </c>
@@ -31686,7 +31685,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="16.5" hidden="1">
+    <row r="151" spans="1:14" ht="16.5">
       <c r="A151" s="96">
         <v>150</v>
       </c>
@@ -31722,7 +31721,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="16.5" hidden="1">
+    <row r="152" spans="1:14" ht="16.5">
       <c r="A152" s="96">
         <v>151</v>
       </c>
@@ -31758,7 +31757,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="16.5" hidden="1">
+    <row r="153" spans="1:14" ht="16.5">
       <c r="A153" s="96">
         <v>152</v>
       </c>
@@ -31794,7 +31793,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="16.5" hidden="1">
+    <row r="154" spans="1:14" ht="16.5">
       <c r="A154" s="96">
         <v>153</v>
       </c>
@@ -31830,7 +31829,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="16.5" hidden="1">
+    <row r="155" spans="1:14" ht="16.5">
       <c r="A155" s="96">
         <v>154</v>
       </c>
@@ -31866,7 +31865,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="16.5" hidden="1">
+    <row r="156" spans="1:14" ht="16.5">
       <c r="A156" s="96">
         <v>155</v>
       </c>
@@ -31902,7 +31901,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="16.5" hidden="1">
+    <row r="157" spans="1:14" ht="16.5">
       <c r="A157" s="96">
         <v>156</v>
       </c>
@@ -31938,7 +31937,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="16.5" hidden="1">
+    <row r="158" spans="1:14" ht="16.5">
       <c r="A158" s="96">
         <v>157</v>
       </c>
@@ -31974,7 +31973,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="16.5" hidden="1">
+    <row r="159" spans="1:14" ht="16.5">
       <c r="A159" s="96">
         <v>158</v>
       </c>
@@ -32010,7 +32009,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="16.5" hidden="1">
+    <row r="160" spans="1:14" ht="16.5">
       <c r="A160" s="96">
         <v>159</v>
       </c>
@@ -32046,7 +32045,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="16.5" hidden="1">
+    <row r="161" spans="1:14" ht="16.5">
       <c r="A161" s="96">
         <v>160</v>
       </c>
@@ -32082,7 +32081,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="16.5" hidden="1">
+    <row r="162" spans="1:14" ht="16.5">
       <c r="A162" s="96">
         <v>161</v>
       </c>
@@ -32118,7 +32117,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="16.5" hidden="1">
+    <row r="163" spans="1:14" ht="16.5">
       <c r="A163" s="96">
         <v>162</v>
       </c>
@@ -32154,7 +32153,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="16.5" hidden="1">
+    <row r="164" spans="1:14" ht="16.5">
       <c r="A164" s="96">
         <v>163</v>
       </c>
@@ -32190,7 +32189,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="16.5" hidden="1">
+    <row r="165" spans="1:14" ht="16.5">
       <c r="A165" s="96">
         <v>164</v>
       </c>
@@ -32226,7 +32225,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="16.5" hidden="1">
+    <row r="166" spans="1:14" ht="16.5">
       <c r="A166" s="96">
         <v>165</v>
       </c>
@@ -32262,7 +32261,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="16.5" hidden="1">
+    <row r="167" spans="1:14" ht="16.5">
       <c r="A167" s="96">
         <v>166</v>
       </c>
@@ -32298,7 +32297,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="16.5" hidden="1">
+    <row r="168" spans="1:14" ht="16.5">
       <c r="A168" s="96">
         <v>167</v>
       </c>
@@ -32334,7 +32333,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="16.5" hidden="1">
+    <row r="169" spans="1:14" ht="16.5">
       <c r="A169" s="96">
         <v>168</v>
       </c>
@@ -32370,7 +32369,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="16.5" hidden="1">
+    <row r="170" spans="1:14" ht="16.5">
       <c r="A170" s="96">
         <v>169</v>
       </c>
@@ -32406,7 +32405,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="16.5" hidden="1">
+    <row r="171" spans="1:14" ht="16.5">
       <c r="A171" s="96">
         <v>170</v>
       </c>
@@ -32442,7 +32441,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="16.5" hidden="1">
+    <row r="172" spans="1:14" ht="16.5">
       <c r="A172" s="96">
         <v>171</v>
       </c>
@@ -32478,7 +32477,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="16.5" hidden="1">
+    <row r="173" spans="1:14" ht="16.5">
       <c r="A173" s="96">
         <v>172</v>
       </c>
@@ -32514,7 +32513,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="16.5" hidden="1">
+    <row r="174" spans="1:14" ht="16.5">
       <c r="A174" s="96">
         <v>173</v>
       </c>
@@ -32550,7 +32549,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="16.5" hidden="1">
+    <row r="175" spans="1:14" ht="16.5">
       <c r="A175" s="96">
         <v>174</v>
       </c>
@@ -32586,7 +32585,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="16.5" hidden="1">
+    <row r="176" spans="1:14" ht="16.5">
       <c r="A176" s="96">
         <v>175</v>
       </c>
@@ -32622,7 +32621,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="16.5" hidden="1">
+    <row r="177" spans="1:14" ht="16.5">
       <c r="A177" s="96">
         <v>176</v>
       </c>
@@ -32658,7 +32657,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="16.5" hidden="1">
+    <row r="178" spans="1:14" ht="16.5">
       <c r="A178" s="96">
         <v>177</v>
       </c>
@@ -32694,7 +32693,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="16.5" hidden="1">
+    <row r="179" spans="1:14" ht="16.5">
       <c r="A179" s="96">
         <v>178</v>
       </c>
@@ -32730,7 +32729,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="16.5" hidden="1">
+    <row r="180" spans="1:14" ht="16.5">
       <c r="A180" s="96">
         <v>179</v>
       </c>
@@ -32766,7 +32765,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="16.5" hidden="1">
+    <row r="181" spans="1:14" ht="16.5">
       <c r="A181" s="96">
         <v>180</v>
       </c>
@@ -32802,7 +32801,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="16.5" hidden="1">
+    <row r="182" spans="1:14" ht="16.5">
       <c r="A182" s="96">
         <v>181</v>
       </c>
@@ -32838,7 +32837,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="16.5" hidden="1">
+    <row r="183" spans="1:14" ht="16.5">
       <c r="A183" s="96">
         <v>182</v>
       </c>
@@ -32874,7 +32873,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="16.5" hidden="1">
+    <row r="184" spans="1:14" ht="16.5">
       <c r="A184" s="96">
         <v>183</v>
       </c>
@@ -32910,7 +32909,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="16.5" hidden="1">
+    <row r="185" spans="1:14" ht="16.5">
       <c r="A185" s="96">
         <v>184</v>
       </c>
@@ -32946,7 +32945,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="16.5" hidden="1">
+    <row r="186" spans="1:14" ht="16.5">
       <c r="A186" s="96">
         <v>185</v>
       </c>
@@ -32982,7 +32981,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="16.5" hidden="1">
+    <row r="187" spans="1:14" ht="16.5">
       <c r="A187" s="96">
         <v>186</v>
       </c>
@@ -33018,7 +33017,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="16.5" hidden="1">
+    <row r="188" spans="1:14" ht="16.5">
       <c r="A188" s="96">
         <v>187</v>
       </c>
@@ -33054,7 +33053,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="16.5" hidden="1">
+    <row r="189" spans="1:14" ht="16.5">
       <c r="A189" s="96">
         <v>188</v>
       </c>
@@ -33090,7 +33089,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="16.5" hidden="1">
+    <row r="190" spans="1:14" ht="16.5">
       <c r="A190" s="96">
         <v>189</v>
       </c>
@@ -33126,7 +33125,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="16.5" hidden="1">
+    <row r="191" spans="1:14" ht="16.5">
       <c r="A191" s="96">
         <v>190</v>
       </c>
@@ -33162,7 +33161,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="16.5" hidden="1">
+    <row r="192" spans="1:14" ht="16.5">
       <c r="A192" s="96">
         <v>191</v>
       </c>
@@ -33198,7 +33197,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="16.5" hidden="1">
+    <row r="193" spans="1:14" ht="16.5">
       <c r="A193" s="96">
         <v>192</v>
       </c>
@@ -33234,7 +33233,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="16.5" hidden="1">
+    <row r="194" spans="1:14" ht="16.5">
       <c r="A194" s="96">
         <v>193</v>
       </c>
@@ -33270,7 +33269,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="16.5" hidden="1">
+    <row r="195" spans="1:14" ht="16.5">
       <c r="A195" s="96">
         <v>194</v>
       </c>
@@ -33306,7 +33305,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="16.5" hidden="1">
+    <row r="196" spans="1:14" ht="16.5">
       <c r="A196" s="96">
         <v>195</v>
       </c>
@@ -33342,7 +33341,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="16.5" hidden="1">
+    <row r="197" spans="1:14" ht="16.5">
       <c r="A197" s="96">
         <v>196</v>
       </c>
@@ -33378,7 +33377,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="16.5" hidden="1">
+    <row r="198" spans="1:14" ht="16.5">
       <c r="A198" s="96">
         <v>197</v>
       </c>
@@ -33414,7 +33413,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="16.5" hidden="1">
+    <row r="199" spans="1:14" ht="16.5">
       <c r="A199" s="96">
         <v>198</v>
       </c>
@@ -33450,7 +33449,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="16.5" hidden="1">
+    <row r="200" spans="1:14" ht="16.5">
       <c r="A200" s="96">
         <v>199</v>
       </c>
@@ -33486,7 +33485,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="16.5" hidden="1">
+    <row r="201" spans="1:14" ht="16.5">
       <c r="A201" s="96">
         <v>200</v>
       </c>
@@ -33522,7 +33521,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="16.5" hidden="1">
+    <row r="202" spans="1:14" ht="16.5">
       <c r="A202" s="96">
         <v>201</v>
       </c>
@@ -33558,7 +33557,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="16.5" hidden="1">
+    <row r="203" spans="1:14" ht="16.5">
       <c r="A203" s="96">
         <v>202</v>
       </c>
@@ -33594,7 +33593,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="16.5" hidden="1">
+    <row r="204" spans="1:14" ht="16.5">
       <c r="A204" s="96">
         <v>203</v>
       </c>
@@ -33630,7 +33629,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="16.5" hidden="1">
+    <row r="205" spans="1:14" ht="16.5">
       <c r="A205" s="96">
         <v>204</v>
       </c>
@@ -33666,7 +33665,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="16.5" hidden="1">
+    <row r="206" spans="1:14" ht="16.5">
       <c r="A206" s="96">
         <v>205</v>
       </c>
@@ -33702,7 +33701,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="16.5" hidden="1">
+    <row r="207" spans="1:14" ht="16.5">
       <c r="A207" s="96">
         <v>206</v>
       </c>
@@ -33738,7 +33737,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="16.5" hidden="1">
+    <row r="208" spans="1:14" ht="16.5">
       <c r="A208" s="96">
         <v>207</v>
       </c>
@@ -33774,7 +33773,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="16.5" hidden="1">
+    <row r="209" spans="1:14" ht="16.5">
       <c r="A209" s="96">
         <v>208</v>
       </c>
@@ -33810,7 +33809,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="16.5" hidden="1">
+    <row r="210" spans="1:14" ht="16.5">
       <c r="A210" s="96">
         <v>209</v>
       </c>
@@ -33846,7 +33845,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="16.5" hidden="1">
+    <row r="211" spans="1:14" ht="16.5">
       <c r="A211" s="96">
         <v>210</v>
       </c>
@@ -33882,7 +33881,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="16.5" hidden="1">
+    <row r="212" spans="1:14" ht="16.5">
       <c r="A212" s="96">
         <v>211</v>
       </c>
@@ -33918,7 +33917,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="16.5" hidden="1">
+    <row r="213" spans="1:14" ht="16.5">
       <c r="A213" s="96">
         <v>212</v>
       </c>
@@ -33954,7 +33953,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="16.5" hidden="1">
+    <row r="214" spans="1:14" ht="16.5">
       <c r="A214" s="96">
         <v>213</v>
       </c>
@@ -33990,7 +33989,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="16.5" hidden="1">
+    <row r="215" spans="1:14" ht="16.5">
       <c r="A215" s="96">
         <v>214</v>
       </c>
@@ -34026,7 +34025,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="16.5" hidden="1">
+    <row r="216" spans="1:14" ht="16.5">
       <c r="A216" s="96">
         <v>215</v>
       </c>
@@ -34062,7 +34061,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="16.5" hidden="1">
+    <row r="217" spans="1:14" ht="16.5">
       <c r="A217" s="96">
         <v>216</v>
       </c>
@@ -34098,7 +34097,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="16.5" hidden="1">
+    <row r="218" spans="1:14" ht="16.5">
       <c r="A218" s="96">
         <v>217</v>
       </c>
@@ -34134,7 +34133,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="16.5" hidden="1">
+    <row r="219" spans="1:14" ht="16.5">
       <c r="A219" s="96">
         <v>218</v>
       </c>
@@ -34170,7 +34169,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="16.5" hidden="1">
+    <row r="220" spans="1:14" ht="16.5">
       <c r="A220" s="96">
         <v>219</v>
       </c>
@@ -34206,7 +34205,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="16.5" hidden="1">
+    <row r="221" spans="1:14" ht="16.5">
       <c r="A221" s="96">
         <v>220</v>
       </c>
@@ -34242,7 +34241,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="16.5" hidden="1">
+    <row r="222" spans="1:14" ht="16.5">
       <c r="A222" s="96">
         <v>221</v>
       </c>
@@ -34278,7 +34277,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="16.5" hidden="1">
+    <row r="223" spans="1:14" ht="16.5">
       <c r="A223" s="96">
         <v>222</v>
       </c>
@@ -34314,7 +34313,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="16.5" hidden="1">
+    <row r="224" spans="1:14" ht="16.5">
       <c r="A224" s="96">
         <v>223</v>
       </c>
@@ -34350,7 +34349,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="16.5" hidden="1">
+    <row r="225" spans="1:14" ht="16.5">
       <c r="A225" s="96">
         <v>224</v>
       </c>
@@ -34386,7 +34385,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="16.5" hidden="1">
+    <row r="226" spans="1:14" ht="16.5">
       <c r="A226" s="96">
         <v>225</v>
       </c>
@@ -34422,7 +34421,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="16.5" hidden="1">
+    <row r="227" spans="1:14" ht="16.5">
       <c r="A227" s="96">
         <v>226</v>
       </c>
@@ -34458,7 +34457,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="16.5" hidden="1">
+    <row r="228" spans="1:14" ht="16.5">
       <c r="A228" s="96">
         <v>227</v>
       </c>
@@ -34494,7 +34493,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="16.5" hidden="1">
+    <row r="229" spans="1:14" ht="16.5">
       <c r="A229" s="96">
         <v>228</v>
       </c>
@@ -34530,7 +34529,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="16.5" hidden="1">
+    <row r="230" spans="1:14" ht="16.5">
       <c r="A230" s="96">
         <v>229</v>
       </c>
@@ -34566,7 +34565,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="16.5" hidden="1">
+    <row r="231" spans="1:14" ht="16.5">
       <c r="A231" s="96">
         <v>230</v>
       </c>
@@ -34602,7 +34601,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="16.5" hidden="1">
+    <row r="232" spans="1:14" ht="16.5">
       <c r="A232" s="96">
         <v>231</v>
       </c>
@@ -34638,7 +34637,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="16.5" hidden="1">
+    <row r="233" spans="1:14" ht="16.5">
       <c r="A233" s="96">
         <v>232</v>
       </c>
@@ -34674,7 +34673,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="16.5" hidden="1">
+    <row r="234" spans="1:14" ht="16.5">
       <c r="A234" s="96">
         <v>233</v>
       </c>
@@ -34710,7 +34709,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="16.5" hidden="1">
+    <row r="235" spans="1:14" ht="16.5">
       <c r="A235" s="96">
         <v>234</v>
       </c>
@@ -34746,7 +34745,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="16.5" hidden="1">
+    <row r="236" spans="1:14" ht="16.5">
       <c r="A236" s="96">
         <v>235</v>
       </c>
@@ -34782,7 +34781,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="16.5" hidden="1">
+    <row r="237" spans="1:14" ht="16.5">
       <c r="A237" s="96">
         <v>236</v>
       </c>
@@ -34818,7 +34817,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="16.5" hidden="1">
+    <row r="238" spans="1:14" ht="16.5">
       <c r="A238" s="96">
         <v>237</v>
       </c>
@@ -34854,7 +34853,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="16.5" hidden="1">
+    <row r="239" spans="1:14" ht="16.5">
       <c r="A239" s="96">
         <v>238</v>
       </c>
@@ -34890,7 +34889,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="16.5" hidden="1">
+    <row r="240" spans="1:14" ht="16.5">
       <c r="A240" s="96">
         <v>239</v>
       </c>
@@ -34926,7 +34925,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="16.5" hidden="1">
+    <row r="241" spans="1:14" ht="16.5">
       <c r="A241" s="96">
         <v>240</v>
       </c>
@@ -34962,7 +34961,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="16.5" hidden="1">
+    <row r="242" spans="1:14" ht="16.5">
       <c r="A242" s="96">
         <v>241</v>
       </c>
@@ -34998,7 +34997,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="16.5" hidden="1">
+    <row r="243" spans="1:14" ht="16.5">
       <c r="A243" s="96">
         <v>242</v>
       </c>
@@ -35034,7 +35033,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="16.5" hidden="1">
+    <row r="244" spans="1:14" ht="16.5">
       <c r="A244" s="96">
         <v>243</v>
       </c>
@@ -35070,7 +35069,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="16.5" hidden="1">
+    <row r="245" spans="1:14" ht="16.5">
       <c r="A245" s="96">
         <v>244</v>
       </c>
@@ -35106,7 +35105,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="16.5" hidden="1">
+    <row r="246" spans="1:14" ht="16.5">
       <c r="A246" s="96">
         <v>245</v>
       </c>
@@ -35142,7 +35141,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="16.5" hidden="1">
+    <row r="247" spans="1:14" ht="16.5">
       <c r="A247" s="96">
         <v>246</v>
       </c>
@@ -35178,7 +35177,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="16.5" hidden="1">
+    <row r="248" spans="1:14" ht="16.5">
       <c r="A248" s="96">
         <v>247</v>
       </c>
@@ -35214,7 +35213,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="16.5" hidden="1">
+    <row r="249" spans="1:14" ht="16.5">
       <c r="A249" s="96">
         <v>248</v>
       </c>
@@ -35250,7 +35249,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="16.5" hidden="1">
+    <row r="250" spans="1:14" ht="16.5">
       <c r="A250" s="96">
         <v>249</v>
       </c>
@@ -35286,7 +35285,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="16.5" hidden="1">
+    <row r="251" spans="1:14" ht="16.5">
       <c r="A251" s="96">
         <v>250</v>
       </c>
@@ -35322,7 +35321,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="16.5" hidden="1">
+    <row r="252" spans="1:14" ht="16.5">
       <c r="A252" s="96">
         <v>251</v>
       </c>
@@ -35358,7 +35357,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="16.5" hidden="1">
+    <row r="253" spans="1:14" ht="16.5">
       <c r="A253" s="96">
         <v>252</v>
       </c>
@@ -35394,7 +35393,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="16.5" hidden="1">
+    <row r="254" spans="1:14" ht="16.5">
       <c r="A254" s="96">
         <v>253</v>
       </c>
@@ -35430,7 +35429,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="16.5" hidden="1">
+    <row r="255" spans="1:14" ht="16.5">
       <c r="A255" s="96">
         <v>254</v>
       </c>
@@ -35466,7 +35465,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="16.5" hidden="1">
+    <row r="256" spans="1:14" ht="16.5">
       <c r="A256" s="96">
         <v>255</v>
       </c>
@@ -35502,7 +35501,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="16.5" hidden="1">
+    <row r="257" spans="1:14" ht="16.5">
       <c r="A257" s="96">
         <v>256</v>
       </c>
@@ -35538,7 +35537,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="16.5" hidden="1">
+    <row r="258" spans="1:14" ht="16.5">
       <c r="A258" s="96">
         <v>257</v>
       </c>
@@ -35574,7 +35573,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="16.5" hidden="1">
+    <row r="259" spans="1:14" ht="16.5">
       <c r="A259" s="96">
         <v>258</v>
       </c>
@@ -35610,7 +35609,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="16.5" hidden="1">
+    <row r="260" spans="1:14" ht="16.5">
       <c r="A260" s="96">
         <v>259</v>
       </c>
@@ -35646,7 +35645,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="16.5" hidden="1">
+    <row r="261" spans="1:14" ht="16.5">
       <c r="A261" s="96">
         <v>260</v>
       </c>
@@ -35682,7 +35681,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="16.5" hidden="1">
+    <row r="262" spans="1:14" ht="16.5">
       <c r="A262" s="96">
         <v>261</v>
       </c>
@@ -35718,7 +35717,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="16.5" hidden="1">
+    <row r="263" spans="1:14" ht="16.5">
       <c r="A263" s="96">
         <v>262</v>
       </c>
@@ -35754,7 +35753,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="16.5" hidden="1">
+    <row r="264" spans="1:14" ht="16.5">
       <c r="A264" s="96">
         <v>263</v>
       </c>
@@ -35790,7 +35789,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="16.5" hidden="1">
+    <row r="265" spans="1:14" ht="16.5">
       <c r="A265" s="96">
         <v>264</v>
       </c>
@@ -35826,7 +35825,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="16.5" hidden="1">
+    <row r="266" spans="1:14" ht="16.5">
       <c r="A266" s="96">
         <v>265</v>
       </c>
@@ -35862,7 +35861,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="16.5" hidden="1">
+    <row r="267" spans="1:14" ht="16.5">
       <c r="A267" s="96">
         <v>266</v>
       </c>
@@ -35898,7 +35897,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="16.5" hidden="1">
+    <row r="268" spans="1:14" ht="16.5">
       <c r="A268" s="96">
         <v>267</v>
       </c>
@@ -35934,7 +35933,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="16.5" hidden="1">
+    <row r="269" spans="1:14" ht="16.5">
       <c r="A269" s="96">
         <v>268</v>
       </c>
@@ -35970,7 +35969,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="16.5" hidden="1">
+    <row r="270" spans="1:14" ht="16.5">
       <c r="A270" s="96">
         <v>269</v>
       </c>
@@ -36006,7 +36005,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="16.5" hidden="1">
+    <row r="271" spans="1:14" ht="16.5">
       <c r="A271" s="96">
         <v>270</v>
       </c>
@@ -36042,7 +36041,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="16.5" hidden="1">
+    <row r="272" spans="1:14" ht="16.5">
       <c r="A272" s="96">
         <v>271</v>
       </c>
@@ -36078,7 +36077,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="16.5" hidden="1">
+    <row r="273" spans="1:14" ht="16.5">
       <c r="A273" s="96">
         <v>272</v>
       </c>
@@ -36114,7 +36113,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="16.5" hidden="1">
+    <row r="274" spans="1:14" ht="16.5">
       <c r="A274" s="96">
         <v>273</v>
       </c>
@@ -36150,7 +36149,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="16.5" hidden="1">
+    <row r="275" spans="1:14" ht="16.5">
       <c r="A275" s="96">
         <v>274</v>
       </c>
@@ -36186,7 +36185,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="16.5" hidden="1">
+    <row r="276" spans="1:14" ht="16.5">
       <c r="A276" s="96">
         <v>275</v>
       </c>
@@ -36222,7 +36221,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="16.5" hidden="1">
+    <row r="277" spans="1:14" ht="16.5">
       <c r="A277" s="96">
         <v>276</v>
       </c>
@@ -36258,7 +36257,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="16.5" hidden="1">
+    <row r="278" spans="1:14" ht="16.5">
       <c r="A278" s="96">
         <v>277</v>
       </c>
@@ -36294,7 +36293,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="16.5" hidden="1">
+    <row r="279" spans="1:14" ht="16.5">
       <c r="A279" s="96">
         <v>278</v>
       </c>
@@ -36330,7 +36329,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="280" spans="1:14" ht="16.5" hidden="1">
+    <row r="280" spans="1:14" ht="16.5">
       <c r="A280" s="96">
         <v>279</v>
       </c>
@@ -36366,7 +36365,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="16.5" hidden="1">
+    <row r="281" spans="1:14" ht="16.5">
       <c r="A281" s="96">
         <v>280</v>
       </c>
@@ -36402,7 +36401,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="282" spans="1:14" ht="16.5" hidden="1">
+    <row r="282" spans="1:14" ht="16.5">
       <c r="A282" s="96">
         <v>281</v>
       </c>
@@ -36438,7 +36437,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="16.5" hidden="1">
+    <row r="283" spans="1:14" ht="16.5">
       <c r="A283" s="96">
         <v>282</v>
       </c>
@@ -36474,7 +36473,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="16.5" hidden="1">
+    <row r="284" spans="1:14" ht="16.5">
       <c r="A284" s="96">
         <v>283</v>
       </c>
@@ -36510,7 +36509,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="16.5" hidden="1">
+    <row r="285" spans="1:14" ht="16.5">
       <c r="A285" s="96">
         <v>284</v>
       </c>
@@ -36546,7 +36545,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="16.5" hidden="1">
+    <row r="286" spans="1:14" ht="16.5">
       <c r="A286" s="96">
         <v>285</v>
       </c>
@@ -36582,7 +36581,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="16.5" hidden="1">
+    <row r="287" spans="1:14" ht="16.5">
       <c r="A287" s="96">
         <v>286</v>
       </c>
@@ -36618,7 +36617,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="16.5" hidden="1">
+    <row r="288" spans="1:14" ht="16.5">
       <c r="A288" s="96">
         <v>287</v>
       </c>
@@ -36654,7 +36653,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="16.5" hidden="1">
+    <row r="289" spans="1:14" ht="16.5">
       <c r="A289" s="96">
         <v>288</v>
       </c>
@@ -36690,7 +36689,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="16.5" hidden="1">
+    <row r="290" spans="1:14" ht="16.5">
       <c r="A290" s="96">
         <v>289</v>
       </c>
@@ -36726,7 +36725,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="16.5" hidden="1">
+    <row r="291" spans="1:14" ht="16.5">
       <c r="A291" s="96">
         <v>290</v>
       </c>
@@ -36762,7 +36761,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="16.5" hidden="1">
+    <row r="292" spans="1:14" ht="16.5">
       <c r="A292" s="96">
         <v>291</v>
       </c>
@@ -36798,7 +36797,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="16.5" hidden="1">
+    <row r="293" spans="1:14" ht="16.5">
       <c r="A293" s="96">
         <v>292</v>
       </c>
@@ -36870,7 +36869,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="16.5" hidden="1">
+    <row r="295" spans="1:14" ht="16.5">
       <c r="A295" s="96">
         <v>294</v>
       </c>
@@ -36906,7 +36905,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="296" spans="1:14" ht="16.5" hidden="1">
+    <row r="296" spans="1:14" ht="16.5">
       <c r="A296" s="96">
         <v>295</v>
       </c>
@@ -36942,7 +36941,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="297" spans="1:14" ht="16.5" hidden="1">
+    <row r="297" spans="1:14" ht="16.5">
       <c r="A297" s="96">
         <v>296</v>
       </c>
@@ -36978,7 +36977,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="16.5" hidden="1">
+    <row r="298" spans="1:14" ht="16.5">
       <c r="A298" s="96">
         <v>297</v>
       </c>
@@ -37014,7 +37013,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="16.5" hidden="1">
+    <row r="299" spans="1:14" ht="16.5">
       <c r="A299" s="96">
         <v>298</v>
       </c>
@@ -37050,7 +37049,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="16.5" hidden="1">
+    <row r="300" spans="1:14" ht="16.5">
       <c r="A300" s="96">
         <v>299</v>
       </c>
@@ -37086,7 +37085,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="16.5" hidden="1">
+    <row r="301" spans="1:14" ht="16.5">
       <c r="A301" s="96">
         <v>300</v>
       </c>
@@ -37122,7 +37121,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="16.5" hidden="1">
+    <row r="302" spans="1:14" ht="16.5">
       <c r="A302" s="96">
         <v>301</v>
       </c>
@@ -37158,7 +37157,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="16.5" hidden="1">
+    <row r="303" spans="1:14" ht="16.5">
       <c r="A303" s="96">
         <v>302</v>
       </c>
@@ -37194,7 +37193,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="16.5" hidden="1">
+    <row r="304" spans="1:14" ht="16.5">
       <c r="A304" s="96">
         <v>303</v>
       </c>
@@ -37230,7 +37229,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="305" spans="1:14" ht="16.5" hidden="1">
+    <row r="305" spans="1:14" ht="16.5">
       <c r="A305" s="96">
         <v>304</v>
       </c>
@@ -37262,7 +37261,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="16.5" hidden="1">
+    <row r="306" spans="1:14" ht="16.5">
       <c r="A306" s="96">
         <v>305</v>
       </c>
@@ -37294,7 +37293,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="16.5" hidden="1">
+    <row r="307" spans="1:14" ht="16.5">
       <c r="A307" s="96">
         <v>306</v>
       </c>
@@ -37326,7 +37325,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="16.5" hidden="1">
+    <row r="308" spans="1:14" ht="16.5">
       <c r="A308" s="96">
         <v>307</v>
       </c>
@@ -37358,7 +37357,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="16.5" hidden="1">
+    <row r="309" spans="1:14" ht="16.5">
       <c r="A309" s="96">
         <v>308</v>
       </c>
@@ -37390,7 +37389,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="16.5" hidden="1">
+    <row r="310" spans="1:14" ht="16.5">
       <c r="A310" s="96">
         <v>309</v>
       </c>
@@ -37422,7 +37421,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="16.5" hidden="1">
+    <row r="311" spans="1:14" ht="16.5">
       <c r="A311" s="96">
         <v>310</v>
       </c>
@@ -37454,7 +37453,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="16.5" hidden="1">
+    <row r="312" spans="1:14" ht="16.5">
       <c r="A312" s="96">
         <v>311</v>
       </c>
@@ -37486,7 +37485,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="313" spans="1:14" ht="16.5" hidden="1">
+    <row r="313" spans="1:14" ht="16.5">
       <c r="A313" s="96">
         <v>312</v>
       </c>
@@ -37518,7 +37517,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="314" spans="1:14" ht="16.5" hidden="1">
+    <row r="314" spans="1:14" ht="16.5">
       <c r="A314" s="96">
         <v>313</v>
       </c>
@@ -37550,7 +37549,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="16.5" hidden="1">
+    <row r="315" spans="1:14" ht="16.5">
       <c r="A315" s="96">
         <v>314</v>
       </c>
@@ -37582,7 +37581,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="16.5" hidden="1">
+    <row r="316" spans="1:14" ht="16.5">
       <c r="A316" s="96">
         <v>315</v>
       </c>
@@ -37614,7 +37613,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="16.5" hidden="1">
+    <row r="317" spans="1:14" ht="16.5">
       <c r="A317" s="96">
         <v>316</v>
       </c>
@@ -37646,7 +37645,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="318" spans="1:14" ht="16.5" hidden="1">
+    <row r="318" spans="1:14" ht="16.5">
       <c r="A318" s="96">
         <v>317</v>
       </c>
@@ -37678,7 +37677,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="319" spans="1:14" ht="16.5" hidden="1">
+    <row r="319" spans="1:14" ht="16.5">
       <c r="A319" s="96">
         <v>318</v>
       </c>
@@ -37710,7 +37709,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="320" spans="1:14" ht="16.5" hidden="1">
+    <row r="320" spans="1:14" ht="16.5">
       <c r="A320" s="96">
         <v>319</v>
       </c>
@@ -37742,7 +37741,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="321" spans="1:14" ht="16.5" hidden="1">
+    <row r="321" spans="1:14" ht="16.5">
       <c r="A321" s="96">
         <v>320</v>
       </c>
@@ -37774,7 +37773,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="322" spans="1:14" ht="16.5" hidden="1">
+    <row r="322" spans="1:14" ht="16.5">
       <c r="A322" s="96">
         <v>321</v>
       </c>
@@ -37806,7 +37805,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="323" spans="1:14" ht="16.5" hidden="1">
+    <row r="323" spans="1:14" ht="16.5">
       <c r="A323" s="96">
         <v>322</v>
       </c>
@@ -37838,7 +37837,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="324" spans="1:14" ht="16.5" hidden="1">
+    <row r="324" spans="1:14" ht="16.5">
       <c r="A324" s="96">
         <v>323</v>
       </c>
@@ -37870,7 +37869,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="325" spans="1:14" ht="16.5" hidden="1">
+    <row r="325" spans="1:14" ht="16.5">
       <c r="A325" s="96">
         <v>324</v>
       </c>
@@ -37902,7 +37901,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="326" spans="1:14" ht="16.5" hidden="1">
+    <row r="326" spans="1:14" ht="16.5">
       <c r="A326" s="96">
         <v>325</v>
       </c>
@@ -37934,7 +37933,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="327" spans="1:14" ht="16.5" hidden="1">
+    <row r="327" spans="1:14" ht="16.5">
       <c r="A327" s="96">
         <v>326</v>
       </c>
@@ -37966,7 +37965,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="328" spans="1:14" ht="16.5" hidden="1">
+    <row r="328" spans="1:14" ht="16.5">
       <c r="A328" s="96">
         <v>327</v>
       </c>
@@ -37998,7 +37997,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="329" spans="1:14" ht="16.5" hidden="1">
+    <row r="329" spans="1:14" ht="16.5">
       <c r="A329" s="96">
         <v>328</v>
       </c>
@@ -38030,7 +38029,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="330" spans="1:14" ht="16.5" hidden="1">
+    <row r="330" spans="1:14" ht="16.5">
       <c r="A330" s="96">
         <v>329</v>
       </c>
@@ -38062,7 +38061,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="331" spans="1:14" ht="16.5" hidden="1">
+    <row r="331" spans="1:14" ht="16.5">
       <c r="A331" s="96">
         <v>330</v>
       </c>
@@ -38094,7 +38093,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="332" spans="1:14" ht="16.5" hidden="1">
+    <row r="332" spans="1:14" ht="16.5">
       <c r="A332" s="96">
         <v>331</v>
       </c>
@@ -38126,7 +38125,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="333" spans="1:14" ht="16.5" hidden="1">
+    <row r="333" spans="1:14" ht="16.5">
       <c r="A333" s="96">
         <v>332</v>
       </c>
@@ -38158,7 +38157,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="334" spans="1:14" ht="16.5" hidden="1">
+    <row r="334" spans="1:14" ht="16.5">
       <c r="A334" s="96">
         <v>333</v>
       </c>
@@ -38190,7 +38189,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="335" spans="1:14" ht="16.5" hidden="1">
+    <row r="335" spans="1:14" ht="16.5">
       <c r="A335" s="96">
         <v>334</v>
       </c>
@@ -38222,7 +38221,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="336" spans="1:14" ht="16.5" hidden="1">
+    <row r="336" spans="1:14" ht="16.5">
       <c r="A336" s="96">
         <v>335</v>
       </c>
@@ -38254,7 +38253,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="16.5" hidden="1">
+    <row r="337" spans="1:14" ht="16.5">
       <c r="A337" s="96">
         <v>336</v>
       </c>
@@ -38284,7 +38283,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="16.5" hidden="1">
+    <row r="338" spans="1:14" ht="16.5">
       <c r="A338" s="96">
         <v>337</v>
       </c>
@@ -38316,7 +38315,7 @@
         <v>5400000</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="16.5" hidden="1">
+    <row r="339" spans="1:14" ht="16.5">
       <c r="A339" s="96">
         <v>338</v>
       </c>
@@ -38348,7 +38347,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="16.5" hidden="1">
+    <row r="340" spans="1:14" ht="16.5">
       <c r="A340" s="96">
         <v>339</v>
       </c>
@@ -38380,7 +38379,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="16.5" hidden="1">
+    <row r="341" spans="1:14" ht="16.5">
       <c r="A341" s="96">
         <v>340</v>
       </c>
@@ -38412,7 +38411,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="16.5" hidden="1">
+    <row r="342" spans="1:14" ht="16.5">
       <c r="A342" s="96">
         <v>341</v>
       </c>
@@ -38444,7 +38443,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="16.5" hidden="1">
+    <row r="343" spans="1:14" ht="16.5">
       <c r="A343" s="96">
         <v>342</v>
       </c>
@@ -38476,7 +38475,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="16.5" hidden="1">
+    <row r="344" spans="1:14" ht="16.5">
       <c r="A344" s="96">
         <v>343</v>
       </c>
@@ -38508,7 +38507,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="16.5" hidden="1">
+    <row r="345" spans="1:14" ht="16.5">
       <c r="A345" s="96">
         <v>344</v>
       </c>
@@ -38541,20 +38540,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P345">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Emeral"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P345"/>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -38562,9 +38556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1377"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -38574,8 +38568,8 @@
     <col min="3" max="3" width="9.42578125" style="97" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="97"/>
     <col min="5" max="5" width="15" style="97" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="97" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" style="97" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" style="97" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="97" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" style="97" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" style="97" bestFit="1" customWidth="1"/>

</xml_diff>